<commit_message>
Actualizo el formato de los archivos de entrega. Ademas modifique el archivo tablas.DB
</commit_message>
<xml_diff>
--- a/Archivos/Informacion_complementaria.xlsx
+++ b/Archivos/Informacion_complementaria.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Martina\Supermercado sql\TP_integrador_Archivos\TP_integrador_Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingunlamedu.sharepoint.com/sites/BasesdeDatosAplicada-Docentes/Documentos compartidos/Docentes/2024/2doCuatrimestre/TP Integrador-Preparacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{A17665B1-38BF-4AE6-9320-B403BF11F0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2FD1914-B373-4D53-9871-D06CFE300126}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">catalogo!$B$1:$B$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="279">
   <si>
     <t>Ciudad</t>
   </si>
@@ -56,6 +57,9 @@
     <t>Mandalay</t>
   </si>
   <si>
+    <t>Reemplazar por</t>
+  </si>
+  <si>
     <t>San Justo</t>
   </si>
   <si>
@@ -74,6 +78,9 @@
     <t>DNI</t>
   </si>
   <si>
+    <t>Legajo/ID</t>
+  </si>
+  <si>
     <t>Direccion</t>
   </si>
   <si>
@@ -95,6 +102,12 @@
     <t>Gerente de sucursal</t>
   </si>
   <si>
+    <t>Línea de producto</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
     <t>Av. de Mayo 791, B1704 Ramos Mejía, Provincia de Buenos Aires</t>
   </si>
   <si>
@@ -114,6 +127,12 @@
   </si>
   <si>
     <t>Jornada completa</t>
+  </si>
+  <si>
+    <t>email personal</t>
+  </si>
+  <si>
+    <t>email empresa</t>
   </si>
   <si>
     <t>Horario</t>
@@ -168,6 +187,9 @@
     <t>Productos</t>
   </si>
   <si>
+    <t>Medio de pago</t>
+  </si>
+  <si>
     <t>Credit card</t>
   </si>
   <si>
@@ -859,31 +881,13 @@
   </si>
   <si>
     <t>Romina	Natalia.PADILLA@superA.com</t>
-  </si>
-  <si>
-    <t>Líneadeproducto</t>
-  </si>
-  <si>
-    <t>Legajo</t>
-  </si>
-  <si>
-    <t>emailpersonal</t>
-  </si>
-  <si>
-    <t>emailempresa</t>
-  </si>
-  <si>
-    <t>Mediodepago</t>
-  </si>
-  <si>
-    <t>Reemplazarpor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1292,34 +1296,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B2:F5" totalsRowShown="0">
-  <autoFilter ref="B2:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11A086A6-598B-47D5-A223-B0DBD96D7514}" name="Tabla1" displayName="Tabla1" ref="B2:F5" totalsRowShown="0">
+  <autoFilter ref="B2:F5" xr:uid="{11A086A6-598B-47D5-A223-B0DBD96D7514}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ciudad"/>
-    <tableColumn id="2" name="Reemplazarpor"/>
-    <tableColumn id="3" name="Direccion"/>
-    <tableColumn id="4" name="Horario" dataDxfId="15"/>
-    <tableColumn id="5" name="Telefono"/>
+    <tableColumn id="1" xr3:uid="{B279F2FA-3A4D-477B-A0B7-5526FBA1CE34}" name="Ciudad"/>
+    <tableColumn id="2" xr3:uid="{BF06278C-AB08-44C6-8E5B-FA0847539AD1}" name="Reemplazar por"/>
+    <tableColumn id="3" xr3:uid="{9516CA9C-D27E-4565-9721-89106345AB3C}" name="direccion"/>
+    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{CADF9AC2-BE7B-44DF-8828-6D257CD1937F}" name="Telefono"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A2:K17" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A2:K17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K17" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A2:K17" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Legajo" dataDxfId="10"/>
-    <tableColumn id="2" name="Nombre" dataDxfId="9"/>
-    <tableColumn id="3" name="Apellido" dataDxfId="8"/>
-    <tableColumn id="4" name="DNI" dataDxfId="7"/>
-    <tableColumn id="5" name="Direccion" dataDxfId="6"/>
-    <tableColumn id="6" name="emailpersonal" dataDxfId="5"/>
-    <tableColumn id="7" name="emailempresa" dataDxfId="4"/>
-    <tableColumn id="8" name="CUIL" dataDxfId="3"/>
-    <tableColumn id="9" name="Cargo" dataDxfId="2"/>
-    <tableColumn id="10" name="Sucursal" dataDxfId="1"/>
-    <tableColumn id="11" name="Turno" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{411F086D-095A-47E3-AE29-CED45684D248}" name="Legajo/ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{3B3CD7CE-C06D-4ABA-A938-43D077DC5A89}" name="Nombre" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{267B687F-55D8-4352-B021-DF57547E7A57}" name="Apellido" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{B9C342F4-9393-4E11-9AEB-F0E0854FA39C}" name="DNI" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{A67FC6FF-FBF8-4973-8847-BA6066866390}" name="Direccion" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{ACEFFA72-CDF5-4532-B64D-1C3A5777FC08}" name="email personal" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{AEAFF176-83C6-4052-A7D4-ADAAA5DDA386}" name="email empresa" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2F5E8EC4-1355-4B97-9F1F-0DB30157F3BA}" name="CUIL" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{190346E5-2F9C-40DF-A153-14119FDF95AF}" name="Cargo" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{891466BD-7C3F-4E42-BF0A-9A36CDBCCB5E}" name="Sucursal" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{FEEA8CDF-571E-4605-90A1-1FBC961AA6F7}" name="Turno" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1621,87 +1625,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58407310-C82B-4707-8E34-0984954EA726}">
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>277</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="30">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="30">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1713,562 +1717,557 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04809A-CB1B-4D46-A903-714B4EC2DF94}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="84.140625" customWidth="1"/>
-    <col min="6" max="6" width="60.7109375" customWidth="1"/>
-    <col min="7" max="7" width="56" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>273</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>274</v>
+        <v>28</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>275</v>
+        <v>29</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>257020</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D3">
         <v>36383025</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>257021</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D4">
         <v>31816587</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>257022</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D5">
         <v>30103258</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>257023</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D6">
         <v>41408274</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>257024</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D7">
         <v>30417854</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>257025</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D8">
         <v>29943254</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>257026</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D9">
         <v>37633159</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>257027</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D10">
         <v>30338745</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>257028</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="D11">
         <v>34605254</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>257029</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D12">
         <v>36508254</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>257030</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D13">
         <v>34636354</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>257031</v>
       </c>
       <c r="B14" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D14">
         <v>33127114</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>257032</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D15">
         <v>39231254</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>257033</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D16">
         <v>30766254</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>257034</v>
       </c>
       <c r="B17" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D17">
         <v>38974125</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F21" s="12"/>
     </row>
   </sheetData>
@@ -2280,50 +2279,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68890E-1A4A-4BA5-B83B-61727FCC66D7}">
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2332,1209 +2327,1209 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932457C5-F4E5-40E2-86CE-923AE54F2BD9}">
   <dimension ref="B1:C149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>272</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
       <c r="C30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3">
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3">
-      <c r="B55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3">
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3">
-      <c r="B57" t="s">
+      <c r="C73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>40</v>
+      </c>
+      <c r="C79" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>37</v>
+      </c>
+      <c r="C86" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>37</v>
+      </c>
+      <c r="C87" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>41</v>
+      </c>
+      <c r="C93" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>34</v>
+      </c>
+      <c r="C94" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>34</v>
+      </c>
+      <c r="C95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C100" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>34</v>
+      </c>
+      <c r="C102" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>42</v>
+      </c>
+      <c r="C105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>37</v>
+      </c>
+      <c r="C110" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C112" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
         <v>36</v>
       </c>
-      <c r="C57" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3">
-      <c r="B58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3">
-      <c r="B59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3">
-      <c r="B60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3">
-      <c r="B61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3">
-      <c r="B62" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3">
-      <c r="B63" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3">
-      <c r="B64" t="s">
+      <c r="C113" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>34</v>
+      </c>
+      <c r="C114" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>44</v>
+      </c>
+      <c r="C115" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>44</v>
+      </c>
+      <c r="C116" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>34</v>
+      </c>
+      <c r="C117" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>34</v>
+      </c>
+      <c r="C119" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C120" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>39</v>
+      </c>
+      <c r="C122" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>39</v>
+      </c>
+      <c r="C123" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>39</v>
+      </c>
+      <c r="C124" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>34</v>
+      </c>
+      <c r="C125" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>39</v>
+      </c>
+      <c r="C126" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>34</v>
+      </c>
+      <c r="C127" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>34</v>
+      </c>
+      <c r="C129" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
         <v>37</v>
       </c>
-      <c r="C64" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65" t="s">
+      <c r="C133" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
         <v>37</v>
       </c>
-      <c r="C65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3">
-      <c r="B67" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3">
-      <c r="B70" t="s">
-        <v>34</v>
-      </c>
-      <c r="C70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3">
-      <c r="B71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3">
-      <c r="B72" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3">
-      <c r="B73" t="s">
-        <v>29</v>
-      </c>
-      <c r="C73" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" t="s">
-        <v>28</v>
-      </c>
-      <c r="C76" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" t="s">
-        <v>34</v>
-      </c>
-      <c r="C77" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78" t="s">
-        <v>33</v>
-      </c>
-      <c r="C78" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3">
-      <c r="B79" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3">
-      <c r="B80" t="s">
-        <v>34</v>
-      </c>
-      <c r="C80" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3">
-      <c r="B81" t="s">
-        <v>34</v>
-      </c>
-      <c r="C81" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3">
-      <c r="B82" t="s">
-        <v>34</v>
-      </c>
-      <c r="C82" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3">
-      <c r="B84" t="s">
-        <v>34</v>
-      </c>
-      <c r="C84" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85" t="s">
-        <v>29</v>
-      </c>
-      <c r="C85" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3">
-      <c r="B86" t="s">
-        <v>31</v>
-      </c>
-      <c r="C86" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3">
-      <c r="B87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88" t="s">
-        <v>28</v>
-      </c>
-      <c r="C88" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3">
-      <c r="B89" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3">
-      <c r="B90" t="s">
-        <v>28</v>
-      </c>
-      <c r="C90" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3">
-      <c r="B91" t="s">
-        <v>28</v>
-      </c>
-      <c r="C91" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3">
-      <c r="B92" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3">
-      <c r="B93" t="s">
-        <v>35</v>
-      </c>
-      <c r="C93" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3">
-      <c r="B94" t="s">
-        <v>28</v>
-      </c>
-      <c r="C94" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3">
-      <c r="B95" t="s">
-        <v>28</v>
-      </c>
-      <c r="C95" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3">
-      <c r="B96" t="s">
-        <v>28</v>
-      </c>
-      <c r="C96" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3">
-      <c r="B97" t="s">
-        <v>28</v>
-      </c>
-      <c r="C97" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3">
-      <c r="B98" t="s">
-        <v>34</v>
-      </c>
-      <c r="C98" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3">
-      <c r="B99" t="s">
-        <v>35</v>
-      </c>
-      <c r="C99" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3">
-      <c r="B100" t="s">
-        <v>28</v>
-      </c>
-      <c r="C100" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3">
-      <c r="B101" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3">
-      <c r="B102" t="s">
-        <v>28</v>
-      </c>
-      <c r="C102" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3">
-      <c r="B103" t="s">
-        <v>29</v>
-      </c>
-      <c r="C103" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3">
-      <c r="B104" t="s">
-        <v>29</v>
-      </c>
-      <c r="C104" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3">
-      <c r="B105" t="s">
+      <c r="C134" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>39</v>
+      </c>
+      <c r="C135" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>34</v>
+      </c>
+      <c r="C136" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>40</v>
+      </c>
+      <c r="C137" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>36</v>
       </c>
-      <c r="C105" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3">
-      <c r="B106" t="s">
-        <v>31</v>
-      </c>
-      <c r="C106" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3">
-      <c r="B107" t="s">
-        <v>31</v>
-      </c>
-      <c r="C107" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3">
-      <c r="B108" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3">
-      <c r="B109" t="s">
-        <v>31</v>
-      </c>
-      <c r="C109" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3">
-      <c r="B110" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3">
-      <c r="B111" t="s">
-        <v>28</v>
-      </c>
-      <c r="C111" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3">
-      <c r="B112" t="s">
-        <v>34</v>
-      </c>
-      <c r="C112" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3">
-      <c r="B113" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3">
-      <c r="B114" t="s">
-        <v>28</v>
-      </c>
-      <c r="C114" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3">
-      <c r="B115" t="s">
-        <v>38</v>
-      </c>
-      <c r="C115" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3">
-      <c r="B116" t="s">
-        <v>38</v>
-      </c>
-      <c r="C116" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3">
-      <c r="B117" t="s">
-        <v>28</v>
-      </c>
-      <c r="C117" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3">
-      <c r="B118" t="s">
-        <v>29</v>
-      </c>
-      <c r="C118" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3">
-      <c r="B119" t="s">
-        <v>28</v>
-      </c>
-      <c r="C119" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3">
-      <c r="B120" t="s">
-        <v>28</v>
-      </c>
-      <c r="C120" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3">
-      <c r="B121" t="s">
-        <v>28</v>
-      </c>
-      <c r="C121" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="122" spans="2:3">
-      <c r="B122" t="s">
-        <v>33</v>
-      </c>
-      <c r="C122" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3">
-      <c r="B123" t="s">
-        <v>33</v>
-      </c>
-      <c r="C123" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="124" spans="2:3">
-      <c r="B124" t="s">
-        <v>33</v>
-      </c>
-      <c r="C124" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="125" spans="2:3">
-      <c r="B125" t="s">
-        <v>28</v>
-      </c>
-      <c r="C125" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3">
-      <c r="B126" t="s">
-        <v>33</v>
-      </c>
-      <c r="C126" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="127" spans="2:3">
-      <c r="B127" t="s">
-        <v>28</v>
-      </c>
-      <c r="C127" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="128" spans="2:3">
-      <c r="B128" t="s">
-        <v>28</v>
-      </c>
-      <c r="C128" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3">
-      <c r="B129" t="s">
-        <v>28</v>
-      </c>
-      <c r="C129" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3">
-      <c r="B130" t="s">
-        <v>28</v>
-      </c>
-      <c r="C130" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3">
-      <c r="B131" t="s">
-        <v>33</v>
-      </c>
-      <c r="C131" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3">
-      <c r="B132" t="s">
-        <v>29</v>
-      </c>
-      <c r="C132" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3">
-      <c r="B133" t="s">
-        <v>31</v>
-      </c>
-      <c r="C133" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3">
-      <c r="B134" t="s">
-        <v>31</v>
-      </c>
-      <c r="C134" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3">
-      <c r="B135" t="s">
-        <v>33</v>
-      </c>
-      <c r="C135" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="136" spans="2:3">
-      <c r="B136" t="s">
-        <v>28</v>
-      </c>
-      <c r="C136" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="137" spans="2:3">
-      <c r="B137" t="s">
-        <v>34</v>
-      </c>
-      <c r="C137" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="138" spans="2:3">
-      <c r="B138" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="139" spans="2:3">
-      <c r="B139" t="s">
-        <v>30</v>
-      </c>
       <c r="C139" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C140" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C141" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C142" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C143" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C144" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C145" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C146" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="147" spans="2:3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C147" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="148" spans="2:3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C148" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="149" spans="2:3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C149" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3543,37 +3538,37 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA0FD82-22EB-4D01-9C8B-5E4AB0436584}">
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3582,16 +3577,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="940421aca186f6b6cf253ceb76bcb39c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4f5da10e60c2eff5832bc3c34d166e5" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -3802,7 +3787,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3811,17 +3796,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664D04EC-A970-41D8-9994-316B682115F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3840,10 +3825,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>